<commit_message>
Updated folder and map in the works.
</commit_message>
<xml_diff>
--- a/Voter_Registration_By_Party_Affiliation_Feb_2019.xlsx
+++ b/Voter_Registration_By_Party_Affiliation_Feb_2019.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\debis\Documents\R_Projects\Final_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{531D5E03-B957-42A4-AE8C-9F0AE11C90DC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{777562E4-157D-411A-A082-B7F016A5D7BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E2773287-0454-4C33-8AEA-9145E6FA57BB}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="7">
   <si>
     <t>Year</t>
   </si>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1E5DB0-6E75-46CC-9570-1B8A0A2884A0}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -942,22 +942,22 @@
     </row>
     <row r="25" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
-        <v>1992</v>
-      </c>
-      <c r="B25" s="2">
-        <v>2672968</v>
-      </c>
-      <c r="C25" s="2">
-        <v>3318565</v>
+        <v>1991</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D25" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E25" s="2">
-        <v>550292</v>
-      </c>
-      <c r="F25" s="2">
-        <v>6541825</v>
+      <c r="E25" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">

</xml_diff>